<commit_message>
[Abraham]: added array in "cargaOrigen".
</commit_message>
<xml_diff>
--- a/src/assets/anexos/Anexo_Lineas_de_Credito_Digital_IFIS.xlsx
+++ b/src/assets/anexos/Anexo_Lineas_de_Credito_Digital_IFIS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/papamactwo/Desktop/Project/BigPuntos/Front/coop-ifi-front-center/src/assets/anexos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9748EBD-7BBA-9F40-A83F-F1FE4D4A521C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{010BAB8A-4D2F-5146-9C26-AB7F319E7B23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="19320" xr2:uid="{34CE6F97-8127-4792-84FB-86D281043B72}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="500" windowWidth="25560" windowHeight="19320" xr2:uid="{34CE6F97-8127-4792-84FB-86D281043B72}"/>
   </bookViews>
   <sheets>
     <sheet name="Clientes" sheetId="1" r:id="rId1"/>
@@ -499,7 +499,7 @@
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>